<commit_message>
updated list of ransomware and US santion list
</commit_message>
<xml_diff>
--- a/Cryptocurrency-Mapping/US-sanction-lists.xlsx
+++ b/Cryptocurrency-Mapping/US-sanction-lists.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E27B251-41CE-4F6D-BEFD-73F9405D0A30}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C9817B-45E6-4BA0-AEC5-090D1D98D06D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8160" yWindow="4190" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="US-sanction-lists" sheetId="1" r:id="rId1"/>

</xml_diff>